<commit_message>
Fixing Atlach-Nacha two-sided card.
</commit_message>
<xml_diff>
--- a/run/overrides.xlsx
+++ b/run/overrides.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="237">
   <si>
     <t xml:space="preserve">databaseId</t>
   </si>
@@ -686,6 +686,51 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;p&gt;&lt;b&gt;If the investigators possess fewer than 3 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues:&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;blockquote&gt;&lt;i&gt;Try as you might, you cannot find the way to the other side of this ocean of tar.&lt;/i&gt;&lt;/blockquote&gt;&lt;/p&gt;&lt;p&gt;Flip this card back over. Come back when you have a greater understanding of this region. This card may be flipped over again when you are ready.&lt;hr&gt;&lt;b&gt;If the investigators possess at least 3 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues:&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;blockquote&gt;&lt;i&gt;You row farther out, into deeper, darker waters, but there is still no sign of any other shore. Under the surface of the black, tarry liquid, you can see a series of glittering stars, like an unknown constellation beckoning you forward. If you didn't know any better, you would think it was a reflection of the sky above, but there is no sky in this dark realm. You lean over the edge of your boat and nearly vomit from the sensation of vertigo that assaults you. It must be hundreds of miles deep, and filled with horrors beyond your imagining. And yet, you know what you must do...&lt;/i&gt;&lt;/blockquote&gt;&lt;/p&gt;&lt;p&gt;The investigators must spend 3 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues, as a group.&lt;/p&gt;&lt;p&gt;Flip this card back over and advance the current act.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atlach-Nacha: The Spider God</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/06/06346a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weaver of the Cosmos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">woc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ancient One. Spider. Elite.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Massive.  &lt;b&gt;Forced&lt;/b&gt; - When Atlach-Nacha leaves a location: If there are no investigators at that location, place 1 doom there. Otherwise, it attacks each investigator at that location.  &lt;b&gt;Forced&lt;/b&gt; - After you evade Atlach-Nacha: Instead of exhausting it, choose an investigator at your location. It cannot attack the chosen investigator this round.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atlach-Nacha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/06/06346b.webp</t>
   </si>
 </sst>
 </file>
@@ -696,7 +741,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -717,6 +762,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -761,12 +811,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -792,29 +846,29 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="20.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="5.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="22.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="4.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="5.04"/>
@@ -842,7 +896,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="4.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="10.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="245.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="295.9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3203,6 +3257,169 @@
       </c>
       <c r="AT31" s="0" t="s">
         <v>221</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="K32" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q32" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="R32" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="S32" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="AA32" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="AB32" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AE32" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="AF32" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="AG32" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="AH32" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="AM32" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="AP32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT32" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="K33" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q33" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="S33" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS33" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Replace … with ... Added Triumph and Subjugation override (missing encounter set).
</commit_message>
<xml_diff>
--- a/run/overrides.xlsx
+++ b/run/overrides.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="243">
   <si>
     <t xml:space="preserve">databaseId</t>
   </si>
@@ -731,6 +731,24 @@
   </si>
   <si>
     <t xml:space="preserve">card_images/06/06346b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Triumph and Subjugation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/90/90023b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad Blood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p&gt;Agnes Baker must decide (choose one):&lt;/p&gt;&lt;p&gt;- Agnes Baker collects 1 memory from Elspeth Baudin.&lt;/p&gt;&lt;p&gt;- Agnes Baker gains 2 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues from the token bank.&lt;/p&gt;&lt;p&gt;Then, flip this card over, exhausted and unengaged.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -741,7 +759,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -762,11 +780,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -820,7 +833,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -846,10 +859,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+      <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.03"/>
@@ -874,16 +887,16 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="5.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="12.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="11.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="9.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="13.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="11.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="6.01"/>
@@ -892,7 +905,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="4.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="10.6"/>
@@ -3420,6 +3433,80 @@
       </c>
       <c r="AS33" s="1" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="K34" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q34" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="S34" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT34" s="0" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
reduced the number of overrides needed after arkhamdb fixes ignore any tsv file copies
</commit_message>
<xml_diff>
--- a/run/overrides.xlsx
+++ b/run/overrides.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="159">
   <si>
     <t xml:space="preserve">databaseId</t>
   </si>
@@ -160,619 +160,316 @@
     <t xml:space="preserve">text</t>
   </si>
   <si>
-    <t xml:space="preserve">06127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cryptic Souls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06127b.webp</t>
+    <t xml:space="preserve">06346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atlach-Nacha: The Spider God</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/06/06346a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">multi_sided</t>
   </si>
   <si>
+    <t xml:space="preserve">Enemy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weaver of the Cosmos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">woc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">346</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mythos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ancient One. Spider. Elite.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Massive.  &lt;b&gt;Forced&lt;/b&gt; - When Atlach-Nacha leaves a location: If there are no investigators at that location, place 1 doom there. Otherwise, it attacks each investigator at that location.  &lt;b&gt;Forced&lt;/b&gt; - After you evade Atlach-Nacha: Instead of exhausting it, choose an investigator at your location. It cannot attack the chosen investigator this round.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atlach-Nacha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/06/06346b.webp</t>
+  </si>
+  <si>
     <t xml:space="preserve">Story</t>
   </si>
   <si>
-    <t xml:space="preserve">The Search for Kadath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sfk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mythos.</t>
-  </si>
-  <si>
     <t xml:space="preserve">B</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;&lt;hr&gt;Check Campaign Log. &lt;i&gt;If the cats collected their tribute from the Zoogs&lt;/i&gt;, read the following:&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;blockquote&gt;&lt;i&gt;One by one, the cats demand a tribute in the form of physical affection. Despite the urgency of your task, they rub against your legs, leap onto your lap, and do not leave until they are thoroughly adored.&lt;/i&gt;&lt;/blockquote&gt;&lt;/p&gt;&lt;p&gt;Lose all of your remaining actions and end your turn.&lt;/p&gt;&lt;p&gt;&lt;hr&gt;&lt;b&gt;&lt;i&gt;If the investigators forced their way into the temple&lt;/i&gt;, read the following:&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;blockquote&gt;&lt;i&gt;The next thing you know, the cats have you completely surrounded. They hiss and growl, closing in from all sides.&lt;/i&gt;&lt;/blockquote&gt;&lt;/p&gt;&lt;p&gt;Spawn the Cats of Ulthar enemy engaged with you.&lt;/p&gt;&lt;p&gt;&lt;hr&gt;&lt;b&gt;Regardless:&lt;/b&gt;&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dreamlike Horrors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06128b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Cancel the effects of the move.&lt;/p&gt;&lt;p&gt;If there are no &lt;b&gt;&lt;i&gt;Creature&lt;/i&gt;&lt;/b&gt; enemies at Skai River, discard cards from the top of the encounter deck until a &lt;b&gt;&lt;i&gt;Creature&lt;/i&gt;&lt;/b&gt; enemy is discarded, and spawn that enemy engaged with you.&lt;/p&gt;&lt;p&gt;Otherwise, add 1 swarm card to a &lt;b&gt;&lt;i&gt;Creature&lt;/i&gt;&lt;/b&gt; enemy at Skai River.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Endless Secrets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06129b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">129</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;You have uncovered a Sign of the Gods &lt;i&gt;(place 1 resource on the scenario reference card to indicate this)&lt;/i&gt;. For the remainder of the scenario, resources on the scenario reference card represent Signs of the Gods the investigators have uncovered. Your quest is to uncover as many of these signs as you can in order to discern the location of Kadath.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06130</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cylinders of Kadatheron</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06130b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">130</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;You have uncovered a Sign of the Gods &lt;i&gt;(place 1 resource on the scenario reference card)&lt;/i&gt;.&lt;/p&gt;&lt;p&gt;Shuffle 1 set-aside copy of Tenebrous Nightgaunt into the encounter deck, if able.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06131</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Doom of Sarnath</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06131b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">131</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;You have uncovered a Sign of the Gods &lt;i&gt;(place 1 resource on the scenario reference card)&lt;/i&gt;.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ghosts of the Dead</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06132b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">132</t>
+    <t xml:space="preserve">87005a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tindalos: Realm of Angular Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87005aa.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machinations Through Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mtt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Past. Present. Future.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tindalos is connected to each [[Portal]] location, and vice versa.  [fast] If it is your turn: Move to a [[Portal]] location.  [action]: Test [combat] (2) or [agility] (2). If you succeed, rescue an abducted [[Scientist]] asset and put it into play at Tindalos, exhausted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tindalos: Maze of Infinite Depths</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87005ab.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epic Multiplayer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tindalos is connected to each [[Portal]] location, and vice versa.  [fast]: Place 1 of your clues on Tindalos, or take control of 1 clue on a Tindalos location in any era.  [action]: Test [combat] (3) or [agility] (3). If you succeed, rescue an abducted [[Scientist]] asset and put it into play at Tindalos, exhausted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Noble Legacy (Past)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87006a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Setup&lt;/b&gt;: Place the Nikola Tesla asset at the [[Past]] River Docks. Flip this story card over.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87006b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[action] If you, Thomas Corrigan, and Mary Zielinski are all at the [[Past]] Miskatonic University: Announce "Thomas and Mary have met."  [action] If Thomas Corrigan, Mary Zielinski, and Nikola Tesla are all at the same location, spend 2 [per_investigator] clues, as a group: Announce "Thomas and Mary are inspired by Nikola Tesla."  [fast] If you are at the [[Past]] Miskatonic University, spend 2 [per_investigator] resources: Announce "funding for an observatory has begun."  &lt;b&gt;Objective&lt;/b&gt; - If all 3 abilities on this story card have been triggered, add it to the victory display &lt;i&gt;(Place a resource token over each ability when it is triggered)&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Noble Legacy (Present)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87015a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
   </si>
   <si>
     <t xml:space="preserve">14</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Remember that the investigators "know what happened to Ib."&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06133</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Palace of Rainbows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06133b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">133</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Each investigator at Ilek-Vad heals 2 horror and draws 2 cards.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06134</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Shrine to the Gods</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06134b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">134</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Crypt of Zulan-Thek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06135b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;You have uncovered a Sign of the Gods &lt;i&gt;(place 1 resource on the scenario reference card)&lt;/i&gt;.&lt;/p&gt;&lt;p&gt;Add Horde of Night to the victory display.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06136</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wares of Baharna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06136b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">136</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Each investigator at Baharna may return an &lt;b&gt;&lt;i&gt;Item&lt;/i&gt;&lt;/b&gt; or &lt;b&gt;&lt;i&gt;Supply&lt;/i&gt;&lt;/b&gt; card from their discard pile to their hand.&lt;/p&gt;&lt;p&gt;Remember that the investigators have "obtained supplies from Baharna."&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06137</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Likeness of Old</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06137b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">137</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What Remains of Tyrrhia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06138b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">138</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06139</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Advice of the King</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06139b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">139</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Remember that you have "beseeched the King."&lt;/p&gt;&lt;p&gt;Shuffle 1 set-aside copy of Tenebrous Nightgaunt into the encounter deck, if able.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06140</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timeless Beauty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06140b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">140</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Each investigator at Serannian heals 2 damage and gains 2 resources.&lt;/p&gt;&lt;p&gt;You have uncovered a Sign of the Gods &lt;i&gt;(place 1 resource on the scenario reference card)&lt;/i&gt;.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unattainable Desires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06141b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">141</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Put the set-aside Temple of Unattainable Desires location into play.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06142</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The City Inside</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06142b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">142</t>
+    <t xml:space="preserve">&lt;b&gt;Setup&lt;/b&gt;: Place the Ezra Graves asset at the [[Present]] Arkham Advertiser. Flip this story card over.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87015b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[action] If you are at the [[Present]] Miskatonic University and "funding for an observatory has begun:" Announce "the observatory is built."  [action] If "the observatory is built," "Thomas and Mary are inspired by Nikola Tesla," and Thomas Corrigan, Mary Zielinski and Ezra Graves are at the [[Present]] Miskatonic University, spend 2 [per_investigator] clues, as a group (4 [per_investigator] clues, as a group, instead if you are playing in &lt;i&gt;Epic Multiplayer Mode&lt;/i&gt;): Announce "teleportation research has begun."  [fast] If "Thomas and Mary have met" and Thomas Corrigan and Mary Zielinski are at Ye Olde Magick Shoppe, spend 1 [per_investigator] resources: Announce "Corrigan Industries has been founded" and put the set-aside Corrigan Industries location into play in the future era.  &lt;b&gt;Objective&lt;/b&gt; - If all 3 abilities on this story card have been triggered, add it to the victory display &lt;i&gt;(place a resource token over each ability when it is triggered)&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Noble Legacy (Future)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87024a.webp</t>
   </si>
   <si>
     <t xml:space="preserve">24</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;p&gt;Put the set-aside City-Which-Appears-On-No-Map location into play.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06143</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Baleful Star</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06143b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">143</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;You have uncovered two Signs of the Gods &lt;i&gt;(place 2 resources on the scenario reference card)&lt;/i&gt;.&lt;/p&gt;&lt;p&gt;Discard each enemy here. Move each investigator here to the Temple of Unattainable Desires (cannot be canceled). Flip this card back over and add it to the victory display.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06214</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Off the Galley</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06214b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dark Side of the Moon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dsm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">214</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;If there were no clues on this card when it was flipped, read the following:&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;i&gt;&lt;blockquote&gt;Moving as stealthily as you can, you find a dinghy tied to the side of the ship, two oars left inside. If this galley can move through space using oars, surely this lifeboat can, too. Making sure to stay as quiet as possible, you hop inside the small boat and make your escape.&lt;/blockquote&gt;&lt;/i&gt;&lt;/p&gt;&lt;p&gt;Move each investigator here to the Moon-Forest.&lt;/p&gt;&lt;p&gt;Remove this card from the game, discarding all enemies here.&lt;hr&gt;&lt;/p&gt;&lt;p&gt;&lt;b&gt;If there were 1 or more clues on this card when it was flipped, read the following:&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;i&gt;&lt;blockquote&gt;The ship docks at a great city of stone towers, and you slip away as the guards search for you.&lt;/blockquote&gt;&lt;/i&gt;Each investigator here raises their alarm level by 1.&lt;/p&gt;&lt;p&gt;Move each investigator here to the City of the Moon-Beasts, along with each enemy here.&lt;/p&gt;&lt;p&gt;Remove this card from the game.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ghastly Tunnels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06254b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Point of No Return</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pnr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">254</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Search the encounter deck and discard pile for a &lt;b&gt;&lt;i&gt;Ghast&lt;/i&gt;&lt;/b&gt; enemy and spawn it here exhausted and with 1 clue on it. Shuffle the encounter deck.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06255</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Sentry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06255b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">255</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Spawn the set-aside Gug Sentinel enemy at this location, with 1 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues on it. Test &lt;span class="icon-agility" title="Agility"&gt;&lt;/span&gt; (3). If you succeed, Gug Sentinel enters play exhausted and unengaged. Otherwise, it enters play engaged with you.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06256</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Another Path</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06256b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">256</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Put the set-aside Enchanted Woods &lt;i&gt;(Stone Trapdoor)&lt;/i&gt; into play, revealed.&lt;/p&gt;&lt;p&gt;Record in your Campaign Log &lt;i&gt;the investigators found a way out of the Underworld&lt;/i&gt;.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06257</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A Strange Ghoul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06257b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">257</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;If the investigators possess fewer than 3 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues:&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;blockquote&gt;&lt;i&gt;Try as you might, you cannot make any headway with the creatures that dwell i this region.&lt;/i&gt;&lt;/blockquote&gt;&lt;/p&gt;&lt;p&gt;Flip this card back over. Come back when you have a greater understanding of this region. This card may be flipped over again when you are ready.&lt;hr&gt;&lt;b&gt;If the investigators possess at least 3 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues:&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;blockquote&gt;&lt;i&gt;Having spent considerable time exploring the upper layer, you understand the ghouls' nature a bit more. They are more welcoming than their kin have been in the past, speaking to you in grunting, monosyllabic English. As you consider your options, you are approached by one of their kind who still wears human clothing. Unlike the rest, he is able to communicate with you perfectly. With an air of authority and wisdom about him, he demands to know why you have come to this place.&lt;/i&gt;&lt;/blockquote&gt;&lt;/p&gt;&lt;p&gt;The investigators must spend 3 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues, as a group.&lt;/p&gt;&lt;p&gt;Advance the current act.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06258</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scouting the Vale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06258b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">258</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Look at the top 2 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; cards of the encounter deck. You may discard up to half of those cards. Return the rest to the top of the encounter deck, in any order.&lt;/p&gt;&lt;p&gt;For the remainder of the game, ignore the text on Crag of the Ghouls.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06259</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Something Below</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06259b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">259</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;If there is no Dhole Tunnel at this location, search the encounter deck and discard pile for a Dhole Tunnel and attach it to this location, if able. Shuffle the encounter deck.&lt;/p&gt;&lt;p&gt;If Slithering Dhole is in play, move it to this location and add 2 clues to it. Otherwise, search the encounter deck, discard pile, and victory display for Slithering Dhole, and spawn it at this location, exhausted and with 2 clues on it.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06260</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inhabitants of the Vale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06260b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">260</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Search the encounter deck and discard pile for a Hunting Nightgaunt and spawn it at Vale of Pnath, exhausted.&lt;/p&gt;&lt;p&gt;Each investigator at Peaks of Thok may draw 2 cards.&lt;/p&gt;&lt;p&gt;Choose any enemy in play and place 2 clues on it.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06261</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Way Out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06261b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">261</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;If the investigators possess fewer than 3 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues:&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;blockquote&gt;&lt;i&gt;Try as you might, you cannot find any way out of the dark, barren vale.&lt;/i&gt;&lt;/blockquote&gt;&lt;/p&gt;&lt;p&gt;Flip this card back over. Come back when you have a greater understanding of this region. This card may be flipped over again when you are ready.&lt;hr&gt;&lt;b&gt;If the investigators possess at least 3 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues:&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;blockquote&gt;&lt;i&gt;You venture out into the dark vale and attempt to map out your surroundings. With the knowledge you have accumulated, you know that the source of the disturbances within the Underworld cannot be in this region. There must be another pathway - perhaps a cavern or tunnel - that leads from the vale to a place even deeper beneath the surface of the Dreamlands. As you approach the great stone wall at the far end of the vale, you pick up a foul scent, like sulfur and tar. You follow the stench until it leads you to a wide hole in the wall.&lt;/i&gt;&lt;/blockquote&gt;&lt;/p&gt;&lt;p&gt;The investigators must spend 3 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues, as a group.&lt;/p&gt;&lt;p&gt;Advance the current act.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06262</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spider-Infested Waters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06262b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">262</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Shuffle the encounter discard pile into the encounter deck and discard cards from the top until a &lt;b&gt;&lt;i&gt;Spider&lt;/i&gt;&lt;/b&gt; enemy is discarded. Spawn that enemy here with 1 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues on it (if it is swarming, place those clues on the host enemy).&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06263</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Still Surface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06263b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">263</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Look at the other side of another copy of Sea of Pitch.&lt;/p&gt;&lt;p&gt;Flip this card back over.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06264</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rolling Pits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06264b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">264</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Set all of the clues from each Sea of Pitch aside.&lt;/p&gt;&lt;p&gt;Discard all other tokens and attachments from each Sea of Pitch.&lt;/p&gt;&lt;p&gt;Flip this card back over and shuffle the positions of each copy of Sea of Pitch so you do not know which is which (investigators and enemies remain at their current position).&lt;/p&gt;&lt;p&gt;Distribute the previously set-aside clues among each copy of Sea of Pitch, as evenly as possible.&lt;/p&gt;&lt;p&gt;Each Sea of Pitch may be flipped over again using their veiled keyword.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06265</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Center of the Sea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06265b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">265</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;&lt;b&gt;If the investigators possess fewer than 3 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues:&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;blockquote&gt;&lt;i&gt;Try as you might, you cannot find the way to the other side of this ocean of tar.&lt;/i&gt;&lt;/blockquote&gt;&lt;/p&gt;&lt;p&gt;Flip this card back over. Come back when you have a greater understanding of this region. This card may be flipped over again when you are ready.&lt;hr&gt;&lt;b&gt;If the investigators possess at least 3 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues:&lt;/b&gt;&lt;/p&gt;&lt;p&gt;&lt;blockquote&gt;&lt;i&gt;You row farther out, into deeper, darker waters, but there is still no sign of any other shore. Under the surface of the black, tarry liquid, you can see a series of glittering stars, like an unknown constellation beckoning you forward. If you didn't know any better, you would think it was a reflection of the sky above, but there is no sky in this dark realm. You lean over the edge of your boat and nearly vomit from the sensation of vertigo that assaults you. It must be hundreds of miles deep, and filled with horrors beyond your imagining. And yet, you know what you must do...&lt;/i&gt;&lt;/blockquote&gt;&lt;/p&gt;&lt;p&gt;The investigators must spend 3 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues, as a group.&lt;/p&gt;&lt;p&gt;Flip this card back over and advance the current act.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06346</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atlach-Nacha: The Spider God</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06346a.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enemy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weaver of the Cosmos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">woc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">346</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ancient One. Spider. Elite.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Massive.  &lt;b&gt;Forced&lt;/b&gt; - When Atlach-Nacha leaves a location: If there are no investigators at that location, place 1 doom there. Otherwise, it attacks each investigator at that location.  &lt;b&gt;Forced&lt;/b&gt; - After you evade Atlach-Nacha: Instead of exhausting it, choose an investigator at your location. It cannot attack the chosen investigator this round.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Atlach-Nacha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/06/06346b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87005a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tindalos: Realm of Angular Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/87/87005aa.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Machinations Through Time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mtt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Single Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Past. Present. Future.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tindalos is connected to each [[Portal]] location, and vice versa.  [fast] If it is your turn: Move to a [[Portal]] location.  [action]: Test [combat] (2) or [agility] (2). If you succeed, rescue an abducted [[Scientist]] asset and put it into play at Tindalos, exhausted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tindalos: Maze of Infinite Depths</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/87/87005ab.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epic Multiplayer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tindalos is connected to each [[Portal]] location, and vice versa.  [fast]: Place 1 of your clues on Tindalos, or take control of 1 clue on a Tindalos location in any era.  [action]: Test [combat] (3) or [agility] (3). If you succeed, rescue an abducted [[Scientist]] asset and put it into play at Tindalos, exhausted.</t>
+    <t xml:space="preserve">&lt;b&gt;Setup&lt;/b&gt;: Set the Dimensional Beam Machine asset aside, out of play. Flip this story card over.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87024b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[action] If Thomas Corrigan and Mary Zielinski are at Corrigan Industries: Put the set-aside Dimensional Beam Machine asset into play under your control &lt;i&gt;(if you are eliminated, set it aside, out of play)&lt;/i&gt;.  [action] If "teleportation research has begun" and Thomas Corrigan, Mary Zielinski, and the Dimensional Beam Machine are at the [[Future]] Miskatonic University: Test [intellect] (3). If you succeed, spend 2 [per_investigator] clues, as a group (8 [per_investigator] clues, as a group, instead if you are playing in &lt;i&gt;Epic Multiplayer Mode&lt;/i&gt;) and announce "Thomas and Mary have made a historic discovery."  [action] If "Thomas and Mary have made a historic discovery" and Thomas Corrigan and Mary Zielinski are at the [[Future]] Arkham Advertiser: Announce "Thomas and Mary have won a Nobel Prize."  &lt;b&gt;Objective&lt;/b&gt; - If all 3 abilities on this story card have been triggered, add it to the victory display &lt;i&gt;(place a resource token over each ability when it is triggered)&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Bitter Rivalry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87033a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machination.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Setup&lt;/b&gt;: Follow the instructions for your relevant era(s), below.&lt;hr&gt;&lt;b&gt;Past&lt;/b&gt;: Set Thoman Corrigan aside, out of play; he has been abducted. Place Mary Zielinski at Arkham Gazette. Set the Edwin Bennet enemy aside, out of play.&lt;hr&gt;&lt;b&gt;Present and Future&lt;/b&gt;: Set Thomas Corrigan and Mary Zielinski aside, out of play; they have been abducted. If you are playing in &lt;i&gt;Epic Multiplayer Mode&lt;/i&gt;, set the Edwin Bennet enemy aside, out of play.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87033b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[action] [action]: Ready and move Edwin Bennet to your location &lt;i&gt;(even if he is in another era)&lt;/i&gt;.  [action] If Edwin Bennet is at your location: &lt;b&gt;Fight&lt;/b&gt;/&lt;b&gt;Evade.&lt;/b&gt; Either attack or attempt to evade Edwin Bennet. If you succeed, spend X clues as a group, where X is the global number of players. Then, place 1 resource on him, as a target. (Group limit once per round.)  &lt;b&gt;Objective&lt;/b&gt; - If Edwin Bennet has 3 targets on him and he is at Tindalos, the forces of Tindalos seize him. Remove Edwin Bennet from the game and add all copies of this story card in each era to the victory display.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redeem a Former Colleague</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87034a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Setup&lt;/b&gt;: Follow the instructions for your relevant era(s), below. Then, flip this story card over.&lt;hr&gt;&lt;b&gt;Past&lt;/b&gt;: Set Mary Zielinski aside, out of play; she has been abducted. Place Thomas Corrigan at Childhood Home. If you are playing in &lt;i&gt;Epic Multiplayer Mode&lt;/i&gt;, set the Edwin Bennet enemy aside, out of play.&lt;hr&gt;&lt;b&gt;Present&lt;/b&gt;: Set Thomas Corrigan and Mary Zielinsky aside, out of play: they have been abducted. Spawn the Edwin Bennet enemy at Miskatonic University.&lt;hr&gt;&lt;b&gt;Future&lt;/b&gt;: Set Thomas Corrigan and Mary Zielinski aside, out of play; they have been abducted. If you are playing in &lt;i&gt;Epic Multiplayer Mode&lt;/i&gt;, set the Edwin Bennet enemy aside, out of play.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87034b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[action] [action]: Ready and move Edwin Bennet to your location &lt;i&gt;(even if he is in another era)&lt;/i&gt;.  [action] If Edwin Bennet is at your location: &lt;b&gt;Parley.&lt;/b&gt; Test [willpower] (3) or [intellect] (3). If you succeed, spend X clues, as a group where X is the global number of players. Then, place 1 resource on him, as a redemption.  &lt;b&gt;Objective&lt;/b&gt; - If Edwin Bennet has 3 or more redemption on him and he is at any Miskatonic University with Thomas Corrigan and Mary Zielinski, he is redeemed. Remove all redemption from him and flip him over. Add all copies of this story card in each era to the victory display.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87035</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uneasy Alliance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87035a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Setup&lt;/b&gt;: Follow the instructions for your relevant era(s), below. Then, flip this story card over.&lt;hr&gt;&lt;b&gt;Past&lt;/b&gt;: Place Thomas Corrigan at Childhood Home. Place Mary Zielinski at O'Malley's Watch Shop. Place the Edwin Bennet asset at Arkham Gazette with 12 clues on him, then remove 3 [per_investigator] clues from him.&lt;hr&gt;&lt;b&gt;Present and Future&lt;/b&gt;: Set Thomas Corrigan and Mary Zielinsky aside, out of play: they have been abducted. If you are playing in &lt;i&gt;Epic Multiplayer Mode&lt;/i&gt;, set the Edwin Bennet asset aside, out of play.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87035b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[action] If Edwin Bennet is at your location and he is ready: &lt;b&gt;Parley.&lt;/b&gt; Place 1 of your clues on him. You may test [intellect] (4). If you succeed, place 1 more of your clues on him. If you fail, exhaust him.  [action]: Ready and move Edwin Bennet to your loaction &lt;i&gt;(even if he is in another era)&lt;/i&gt;.  &lt;b&gt;Forced&lt;/b&gt; - At the end of the round: Remove 1 clue from Edwin Bennet (2 clues instead if you are playing in &lt;i&gt;Epic Multiplayer Mode&lt;/i&gt;). If you cannot, place 1 doom on the current agenda. This effect can cause the current agenda to advance.  &lt;b&gt;Forced&lt;/b&gt; - When Edwin Bennet would be abducted: Remove all damage and horror from him and place 2 doom on the current agenda instead.  &lt;b&gt;Objective&lt;/b&gt; - If "Thomas and Mary have won a Nobel Prize" and there is no [[Plot]] story card in play in any era, add this story card to the victory display.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anomalies in Spacetime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87038a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plot.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Setup&lt;/b&gt;: Place 1 [per_investigator] horror on each Miskatonic University location, as anomalies. If you are playing in &lt;i&gt;Epic Multiplayer Mode&lt;/i&gt;, also place 1 [per_investigator] horror on the following locations, as anomalies: Arkham Gazette, Arkham Advertiser, O'Malley's Watch Shop, and Tick-Tock Club.  Remove the following enemies from the game: Tyr'thrha, Old Sadie Sheldon, and all 3 copies of Sheldon Gang. Flip this story card over.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87038b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abilities on locations with an anomaly cannot be triggered.  [action] Spend any number of clues: Test [willpower] (3) or [agility] (3). You get +3 skill value to this test for each clue spent this way. If you succeed, remove 1 anomaly from your location (2 anomalies instead if you succeed by 3 or more). Then, if you succeed by 4 or more and "Corrigan Industries has been founded," remove 1 anomaly from a location with the same title as your location, in any era.  &lt;b&gt;Objective&lt;/b&gt; - If it is agenda 2a and each location has no anomalies, add this story card to the victory display.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mob Troubles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87039a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Setup&lt;/b&gt;: Set the Old Sadie Sheldon enemy and all 3 copies of the Sheldon Gang enemy aside, out of play. Remove the Tyr'thrha enemy from the game. You make a deal with Old Sadie Sheldon: each investigator playing the present era gains 2 resources.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87039b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[action] If "the debt has been paid," spend 1 [per_investigator] clues, as a group: Search the play area, encounter deck, or encounter discard pile for a Sheldon Gang enemy and add it to the victory display. If you searched the encounter deck, shuffle it. This action does not cause attacks of opportunity.  &lt;b&gt;Objective&lt;/b&gt; - If all 3 Sheldon Gang enemies are in the victory display, add this story card to the victory display.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unspeakable Abomination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87042a.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;b&gt;Setup&lt;/b&gt;: Set the Tyr'thrha enemy aside, out of play. Remove the Old Sadie Sheldon enemy and all 3 copies of the Sheldon Gang enemy from the game.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card_images/87/87042b.webp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[action] If Tyr'thrha is at your location, spend 1 clue: Test [intellect] (3). If you succeed, deal 2 damage to Tyr'thrha (3 damage instead if you succeed by 3 or more). This action does not provoke attacks of opportunity.  &lt;b&gt;Objective&lt;/b&gt; - If Tyr'thrha is defeated, add this story card to the victory display.</t>
   </si>
   <si>
     <t xml:space="preserve">89005</t>
@@ -800,24 +497,6 @@
   </si>
   <si>
     <t xml:space="preserve">- &lt;b&gt;-6&lt;/b&gt;: ...all events from each investigator's hand.  - &lt;b&gt;-7&lt;/b&gt;: ...a non-story, non-weakness asset from each investigator's play area.  - &lt;b&gt;-8&lt;/b&gt;: ...a non-weakness siganture card in any player's deck, hand, discard pile, or play area.  - [skull]: ...1 card beneath Ravenous, at random.  - [cultist]: ...each card committed to each skill test at your location &lt;i&gt;(after the test ends)&lt;/i&gt;, until the end of the next investigation phase.  - [tablet]: ...each event played by investigators at your location, until the end of the next investigation phase.  - [elder_thing]: ...the player card at your location with the most evidence, supplies, ammo, charges, or secrets on it.  - [auto_fail]: Reveal 3 more chaos tokens and resolve each of those devour effects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Triumph and Subjugation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">card_images/90/90023b.webp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bad Blood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p&gt;Agnes Baker must decide (choose one):&lt;/p&gt;&lt;p&gt;- Agnes Baker collects 1 memory from Elspeth Baudin.&lt;/p&gt;&lt;p&gt;- Agnes Baker gains 2 &lt;span class="icon-per_investigator" title="Per Investigator"&gt;&lt;/span&gt; clues from the token bank.&lt;/p&gt;&lt;p&gt;Then, flip this card over, exhausted and unengaged.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -893,7 +572,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -907,14 +586,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1041,7 +712,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AT1004"/>
+  <dimension ref="A1:AT991"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1061,7 +732,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="23.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="10.06"/>
@@ -1274,7 +945,7 @@
         <v>55</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>52</v>
@@ -1286,16 +957,34 @@
         <v>52</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>52</v>
+      <c r="AE2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="AP2" s="2" t="s">
         <v>52</v>
@@ -1310,24 +999,24 @@
         <v>52</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>51</v>
@@ -1339,16 +1028,16 @@
         <v>53</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>51</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>52</v>
@@ -1360,10 +1049,10 @@
         <v>52</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="AB3" s="2" t="s">
         <v>52</v>
@@ -1383,43 +1072,41 @@
       <c r="AS3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AT3" s="1" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>67</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>51</v>
+      <c r="E4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>53</v>
+      <c r="I4" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>51</v>
+        <v>73</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>52</v>
@@ -1433,141 +1120,192 @@
       <c r="P4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="3"/>
+      <c r="AP4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL4" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP4" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AQ4" s="2" t="s">
         <v>52</v>
       </c>
       <c r="AR4" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AS4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AT4" s="1" t="s">
-        <v>70</v>
+      <c r="AT4" s="3" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>73</v>
+      <c r="A5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>51</v>
+      <c r="E5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>53</v>
+      <c r="I5" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>51</v>
+        <v>73</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="L5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="R5" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q5" s="1" t="s">
+      <c r="S5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL5" s="3"/>
+      <c r="AM5" s="3"/>
+      <c r="AN5" s="3"/>
+      <c r="AO5" s="3"/>
+      <c r="AP5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="S5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP5" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AQ5" s="2" t="s">
         <v>52</v>
       </c>
       <c r="AR5" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AS5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AT5" s="1" t="s">
-        <v>76</v>
+      <c r="AT5" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="M6" s="2" t="s">
         <v>52</v>
@@ -1582,17 +1320,14 @@
         <v>52</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AB6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AL6" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP6" s="2" t="s">
         <v>52</v>
       </c>
@@ -1606,190 +1341,184 @@
         <v>52</v>
       </c>
       <c r="AT6" s="1" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="L7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AS7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT7" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT7" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L8" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AQ8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AS8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT8" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT8" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>52</v>
@@ -1804,66 +1533,63 @@
         <v>52</v>
       </c>
       <c r="Q9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="S9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP9" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AQ9" s="2" t="s">
         <v>52</v>
       </c>
       <c r="AR9" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AS9" s="2" t="s">
         <v>52</v>
       </c>
       <c r="AT9" s="1" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>104</v>
+        <v>55</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>52</v>
@@ -1878,17 +1604,14 @@
         <v>52</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AB10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AL10" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP10" s="2" t="s">
         <v>52</v>
       </c>
@@ -1902,42 +1625,42 @@
         <v>52</v>
       </c>
       <c r="AT10" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>52</v>
@@ -1952,19 +1675,16 @@
         <v>52</v>
       </c>
       <c r="Q11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="S11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB11" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL11" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP11" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AQ11" s="2" t="s">
         <v>52</v>
@@ -1976,42 +1696,42 @@
         <v>52</v>
       </c>
       <c r="AT11" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>52</v>
@@ -2026,17 +1746,17 @@
         <v>52</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AB12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AL12" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP12" s="2" t="s">
         <v>52</v>
       </c>
@@ -2050,42 +1770,42 @@
         <v>52</v>
       </c>
       <c r="AT12" s="1" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>52</v>
@@ -2100,19 +1820,16 @@
         <v>52</v>
       </c>
       <c r="Q13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="S13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL13" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP13" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AQ13" s="2" t="s">
         <v>52</v>
@@ -2124,42 +1841,42 @@
         <v>52</v>
       </c>
       <c r="AT13" s="1" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>52</v>
@@ -2174,17 +1891,17 @@
         <v>52</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AB14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AL14" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP14" s="2" t="s">
         <v>52</v>
       </c>
@@ -2198,42 +1915,42 @@
         <v>52</v>
       </c>
       <c r="AT14" s="1" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="M15" s="2" t="s">
         <v>52</v>
@@ -2248,19 +1965,16 @@
         <v>52</v>
       </c>
       <c r="Q15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM15" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="S15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL15" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP15" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AQ15" s="2" t="s">
         <v>52</v>
@@ -2272,42 +1986,42 @@
         <v>52</v>
       </c>
       <c r="AT15" s="1" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>52</v>
@@ -2322,17 +2036,17 @@
         <v>52</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AB16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AL16" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP16" s="2" t="s">
         <v>52</v>
       </c>
@@ -2346,42 +2060,42 @@
         <v>52</v>
       </c>
       <c r="AT16" s="1" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>52</v>
@@ -2396,19 +2110,16 @@
         <v>52</v>
       </c>
       <c r="Q17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM17" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="S17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL17" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP17" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AQ17" s="2" t="s">
         <v>52</v>
@@ -2420,42 +2131,42 @@
         <v>52</v>
       </c>
       <c r="AT17" s="1" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>52</v>
@@ -2470,17 +2181,17 @@
         <v>52</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AB18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AL18" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP18" s="2" t="s">
         <v>52</v>
       </c>
@@ -2494,42 +2205,42 @@
         <v>52</v>
       </c>
       <c r="AT18" s="1" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>155</v>
+        <v>71</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>156</v>
+        <v>72</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>155</v>
+        <v>71</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>52</v>
@@ -2544,19 +2255,16 @@
         <v>52</v>
       </c>
       <c r="Q19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM19" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="S19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL19" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP19" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AQ19" s="2" t="s">
         <v>52</v>
@@ -2568,42 +2276,42 @@
         <v>52</v>
       </c>
       <c r="AT19" s="1" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>162</v>
+        <v>71</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>163</v>
+        <v>72</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>162</v>
+        <v>71</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>52</v>
@@ -2618,17 +2326,17 @@
         <v>52</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AB20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AL20" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP20" s="2" t="s">
         <v>52</v>
       </c>
@@ -2642,42 +2350,42 @@
         <v>52</v>
       </c>
       <c r="AT20" s="1" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>169</v>
+        <v>140</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>162</v>
+        <v>71</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>163</v>
+        <v>72</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>170</v>
+        <v>137</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>162</v>
+        <v>71</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>52</v>
@@ -2692,19 +2400,16 @@
         <v>52</v>
       </c>
       <c r="Q21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM21" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="S21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL21" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP21" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AQ21" s="2" t="s">
         <v>52</v>
@@ -2716,42 +2421,42 @@
         <v>52</v>
       </c>
       <c r="AT21" s="1" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>162</v>
+        <v>71</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>163</v>
+        <v>72</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>162</v>
+        <v>71</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>63</v>
+        <v>146</v>
       </c>
       <c r="M22" s="2" t="s">
         <v>52</v>
@@ -2766,17 +2471,17 @@
         <v>52</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AB22" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AL22" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP22" s="2" t="s">
         <v>52</v>
       </c>
@@ -2790,42 +2495,42 @@
         <v>52</v>
       </c>
       <c r="AT22" s="1" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>162</v>
+        <v>71</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>52</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>163</v>
+        <v>72</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>162</v>
+        <v>71</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="M23" s="2" t="s">
         <v>52</v>
@@ -2840,19 +2545,16 @@
         <v>52</v>
       </c>
       <c r="Q23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM23" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="S23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB23" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL23" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP23" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="AQ23" s="2" t="s">
         <v>52</v>
@@ -2864,42 +2566,36 @@
         <v>52</v>
       </c>
       <c r="AT23" s="1" t="s">
-        <v>181</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>184</v>
+        <v>150</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>162</v>
+      <c r="E24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>163</v>
+        <v>56</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>52</v>
@@ -2913,18 +2609,15 @@
       <c r="P24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="Q24" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>57</v>
+      <c r="Q24" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="AB24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AL24" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP24" s="2" t="s">
         <v>52</v>
       </c>
@@ -2937,43 +2630,37 @@
       <c r="AS24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AT24" s="1" t="s">
-        <v>186</v>
+      <c r="AT24" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>189</v>
+        <v>150</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>162</v>
+      <c r="E25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>163</v>
+        <v>56</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>52</v>
@@ -2987,18 +2674,15 @@
       <c r="P25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="Q25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>57</v>
+      <c r="Q25" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="S25" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="AB25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AL25" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="AP25" s="2" t="s">
         <v>52</v>
       </c>
@@ -3011,1020 +2695,48 @@
       <c r="AS25" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AT25" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q26" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT26" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT27" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT28" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q29" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S29" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT29" s="1" t="s">
-        <v>211</v>
+      <c r="AT25" s="3" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S30" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS30" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT30" s="1" t="s">
-        <v>216</v>
-      </c>
+      <c r="A30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q31" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S31" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS31" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT31" s="1" t="s">
-        <v>221</v>
-      </c>
+      <c r="A31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="N32" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O32" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P32" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="S32" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="AA32" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="AB32" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="AE32" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="AF32" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="AG32" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="AH32" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="AM32" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="AP32" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ32" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR32" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS32" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT32" s="1" t="s">
-        <v>234</v>
-      </c>
+      <c r="A32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q33" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S33" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR33" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS33" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="A33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="K34" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="N34" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O34" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="P34" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q34" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="R34" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="S34" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="T34" s="4"/>
-      <c r="U34" s="4"/>
-      <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
-      <c r="X34" s="4"/>
-      <c r="Y34" s="4"/>
-      <c r="Z34" s="4"/>
-      <c r="AA34" s="4"/>
-      <c r="AB34" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC34" s="4"/>
-      <c r="AD34" s="4"/>
-      <c r="AE34" s="4"/>
-      <c r="AF34" s="4"/>
-      <c r="AG34" s="4"/>
-      <c r="AH34" s="4"/>
-      <c r="AI34" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="AJ34" s="4"/>
-      <c r="AK34" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL34" s="4"/>
-      <c r="AM34" s="4"/>
-      <c r="AN34" s="4"/>
-      <c r="AO34" s="4"/>
-      <c r="AP34" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AQ34" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR34" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AS34" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT34" s="4" t="s">
-        <v>246</v>
-      </c>
+      <c r="A34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="N35" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="O35" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="P35" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q35" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="R35" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="S35" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="T35" s="4"/>
-      <c r="U35" s="4"/>
-      <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-      <c r="X35" s="4"/>
-      <c r="Y35" s="4"/>
-      <c r="Z35" s="4"/>
-      <c r="AA35" s="4"/>
-      <c r="AB35" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC35" s="4"/>
-      <c r="AD35" s="4"/>
-      <c r="AE35" s="4"/>
-      <c r="AF35" s="4"/>
-      <c r="AG35" s="4"/>
-      <c r="AH35" s="4"/>
-      <c r="AI35" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="AJ35" s="4"/>
-      <c r="AK35" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL35" s="4"/>
-      <c r="AM35" s="4"/>
-      <c r="AN35" s="4"/>
-      <c r="AO35" s="4"/>
-      <c r="AP35" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AQ35" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR35" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="AS35" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT35" s="4" t="s">
-        <v>250</v>
-      </c>
+      <c r="A35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N36" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O36" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P36" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q36" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="S36" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="AB36" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP36" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ36" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR36" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS36" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT36" s="3" t="s">
-        <v>257</v>
-      </c>
+      <c r="A36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N37" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O37" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q37" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="S37" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB37" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP37" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ37" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR37" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS37" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT37" s="3" t="s">
-        <v>259</v>
-      </c>
+      <c r="A37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I38" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="O38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q38" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S38" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AP38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AQ38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AS38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT38" s="1" t="s">
-        <v>265</v>
-      </c>
+      <c r="A38" s="2"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
@@ -4359,45 +3071,45 @@
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="2"/>
     </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="2"/>
-    </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="2"/>
-    </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="2"/>
-    </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="2"/>
-    </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="2"/>
-    </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="2"/>
-    </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="2"/>
-    </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="2"/>
-    </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="2"/>
-    </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="2"/>
-    </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="2"/>
-    </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="2"/>
-    </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="2"/>
     </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="2"/>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="2"/>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="2"/>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="2"/>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="2"/>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="2"/>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="2"/>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="2"/>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="2"/>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="2"/>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="2"/>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="2"/>
+    </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="2"/>
     </row>
@@ -4757,42 +3469,55 @@
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="2"/>
+      <c r="J298" s="2"/>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="2"/>
+      <c r="J299" s="2"/>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="2"/>
+      <c r="J300" s="2"/>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="2"/>
+      <c r="J301" s="2"/>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="2"/>
+      <c r="J302" s="2"/>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="2"/>
+      <c r="J303" s="2"/>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="2"/>
+      <c r="J304" s="2"/>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="2"/>
+      <c r="J305" s="2"/>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="2"/>
+      <c r="J306" s="2"/>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="2"/>
+      <c r="J307" s="2"/>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="2"/>
+      <c r="J308" s="2"/>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="2"/>
+      <c r="J309" s="2"/>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="2"/>
+      <c r="J310" s="2"/>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="2"/>
@@ -5064,55 +3789,42 @@
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="2"/>
-      <c r="J378" s="2"/>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="2"/>
-      <c r="J379" s="2"/>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="2"/>
-      <c r="J380" s="2"/>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="2"/>
-      <c r="J381" s="2"/>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="2"/>
-      <c r="J382" s="2"/>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="2"/>
-      <c r="J383" s="2"/>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="2"/>
-      <c r="J384" s="2"/>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="2"/>
-      <c r="J385" s="2"/>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="2"/>
-      <c r="J386" s="2"/>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="2"/>
-      <c r="J387" s="2"/>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="2"/>
-      <c r="J388" s="2"/>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="2"/>
-      <c r="J389" s="2"/>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="2"/>
-      <c r="J390" s="2"/>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="2"/>
@@ -5237,44 +3949,44 @@
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="2"/>
     </row>
-    <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A432" s="2"/>
-    </row>
-    <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A433" s="2"/>
-    </row>
-    <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A434" s="2"/>
-    </row>
-    <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A435" s="2"/>
-    </row>
-    <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A436" s="2"/>
-    </row>
-    <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A437" s="2"/>
-    </row>
-    <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A438" s="2"/>
-    </row>
-    <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A439" s="2"/>
-    </row>
-    <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A440" s="2"/>
-    </row>
-    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A441" s="2"/>
-    </row>
-    <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A442" s="2"/>
-    </row>
-    <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A443" s="2"/>
-    </row>
-    <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A444" s="2"/>
+    <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A530" s="2"/>
+    </row>
+    <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A531" s="2"/>
+    </row>
+    <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A532" s="2"/>
+    </row>
+    <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A533" s="2"/>
+    </row>
+    <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A534" s="2"/>
+    </row>
+    <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A535" s="2"/>
+    </row>
+    <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A536" s="2"/>
+    </row>
+    <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A537" s="2"/>
+    </row>
+    <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A538" s="2"/>
+    </row>
+    <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A539" s="2"/>
+    </row>
+    <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A540" s="2"/>
+    </row>
+    <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A541" s="2"/>
+    </row>
+    <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A542" s="2"/>
     </row>
     <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A543" s="2"/>
@@ -6622,45 +5334,6 @@
     </row>
     <row r="991" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A991" s="2"/>
-    </row>
-    <row r="992" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A992" s="2"/>
-    </row>
-    <row r="993" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A993" s="2"/>
-    </row>
-    <row r="994" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A994" s="2"/>
-    </row>
-    <row r="995" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A995" s="2"/>
-    </row>
-    <row r="996" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A996" s="2"/>
-    </row>
-    <row r="997" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A997" s="2"/>
-    </row>
-    <row r="998" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A998" s="2"/>
-    </row>
-    <row r="999" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A999" s="2"/>
-    </row>
-    <row r="1000" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1000" s="2"/>
-    </row>
-    <row r="1001" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1001" s="2"/>
-    </row>
-    <row r="1002" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1002" s="2"/>
-    </row>
-    <row r="1003" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1003" s="2"/>
-    </row>
-    <row r="1004" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1004" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>